<commit_message>
loosely organize components into groups based on their functionality
</commit_message>
<xml_diff>
--- a/profitability.xlsx
+++ b/profitability.xlsx
@@ -15,12 +15,28 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>Unit Sales</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -34,7 +50,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,14 +58,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -349,12 +377,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>